<commit_message>
Added data warngling changes
</commit_message>
<xml_diff>
--- a/tables/table_1.xlsx
+++ b/tables/table_1.xlsx
@@ -14,9 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Year</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Ethics and integrity</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>Corporate governance</t>
@@ -422,159 +428,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1.4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
         <v>1.5</v>
       </c>
-      <c r="C1">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
         <v>1.6</v>
       </c>
-      <c r="D1">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
         <v>2.1</v>
       </c>
-      <c r="F1">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
         <v>2.2</v>
       </c>
-      <c r="G1">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
         <v>2.3</v>
       </c>
-      <c r="H1">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
         <v>2.4</v>
       </c>
-      <c r="I1">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
         <v>3</v>
       </c>
-      <c r="J1">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
         <v>3.1</v>
       </c>
-      <c r="K1">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
         <v>3.2</v>
       </c>
-      <c r="L1">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
         <v>3.3</v>
       </c>
-      <c r="M1">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
         <v>3.4</v>
       </c>
-      <c r="N1">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
         <v>3.5</v>
       </c>
-      <c r="O1">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
         <v>3.6</v>
       </c>
-      <c r="P1">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="1">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>17</v>
-      </c>
-      <c r="E3">
-        <v>17</v>
-      </c>
-      <c r="F3">
-        <v>21</v>
-      </c>
-      <c r="G3">
-        <v>22</v>
-      </c>
-      <c r="H3">
-        <v>24</v>
-      </c>
-      <c r="I3">
-        <v>25</v>
-      </c>
-      <c r="J3">
-        <v>25</v>
-      </c>
-      <c r="K3">
-        <v>26</v>
-      </c>
-      <c r="L3">
-        <v>27</v>
-      </c>
-      <c r="M3">
-        <v>27</v>
-      </c>
-      <c r="N3">
-        <v>29</v>
-      </c>
-      <c r="O3">
-        <v>30</v>
-      </c>
-      <c r="P3">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
         <v>30</v>
       </c>
     </row>

</xml_diff>